<commit_message>
Fix a bug to allow user can rent the car in the empty period
</commit_message>
<xml_diff>
--- a/Testcases.xlsx
+++ b/Testcases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jluo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jluo/Github/car-rental-demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="89">
   <si>
     <t>Test Suite ID</t>
   </si>
@@ -332,9 +332,6 @@
     <t>TC007</t>
   </si>
   <si>
-    <t>To if the rent car is still available</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Login
 2. Select rent date
 3. Select return date
@@ -350,6 +347,34 @@
   </si>
   <si>
     <t>Only show 3 cars</t>
+  </si>
+  <si>
+    <t>To verify if the rent car is still available</t>
+  </si>
+  <si>
+    <t>TC008</t>
+  </si>
+  <si>
+    <t>To verify if the rent car is avaible between two different rent period</t>
+  </si>
+  <si>
+    <t>period1:
+rent date: 20191210
+return date: 20191215
+period2:
+rent date: 20191220
+return date:20191225
+new rent period:
+rent date:20191216
+return date:20191219</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Require to fix the defect
+Update:
+Fixed the defect by introducing a new table rentRecord to keep the rental history</t>
   </si>
 </sst>
 </file>
@@ -482,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -503,6 +528,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -831,11 +859,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -849,11 +877,11 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" ht="230.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -880,11 +908,11 @@
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -1176,10 +1204,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1195,7 +1223,7 @@
     <col min="9" max="9" width="31" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.83203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" style="1" customWidth="1"/>
     <col min="13" max="13" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -1542,7 +1570,7 @@
         <v>47</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>76</v>
@@ -1586,7 +1614,7 @@
         <v>79</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>18</v>
@@ -1595,16 +1623,16 @@
         <v>47</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>76</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K8" s="8" t="s">
         <v>48</v>
@@ -1625,6 +1653,59 @@
         <v>43820</v>
       </c>
       <c r="Q8" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="210" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="7">
+        <v>43821</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="P9" s="7">
+        <v>43821</v>
+      </c>
+      <c r="Q9" s="9" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>